<commit_message>
Corrected equations and intra-models information. Jupyter notebook 12 not showing correct results.
</commit_message>
<xml_diff>
--- a/andes/cases/local/1_inv_1_load.xlsx
+++ b/andes/cases/local/1_inv_1_load.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscar/Documents/heila/tools/andes/andes/cases/local/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscar/Documents/heila/tools/andes-heila/andes/cases/local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD43AADD-0628-1E48-8571-8F0A71D045FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347CF0FA-73CD-944F-AEBE-BFDAC83AFBCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{C773AEB6-E21B-E644-860F-783A0871B2E2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="4" xr2:uid="{C773AEB6-E21B-E644-860F-783A0871B2E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="H3" sqref="H3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.57025491716260168</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -679,10 +679,10 @@
         <v>0.9</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0.99761</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.36874618304434781</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -710,7 +710,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,13 +764,13 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <v>480</v>
+        <v>0.48</v>
       </c>
       <c r="G2">
-        <v>11.59</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>-0.73499999999999999</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>1.1000000000000001</v>
@@ -795,7 +795,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,7 +928,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,10 +1039,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="L2">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1079,7 +1079,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>